<commit_message>
upload readme and Manual
</commit_message>
<xml_diff>
--- a/ver6/Input.xlsx
+++ b/ver6/Input.xlsx
@@ -8,31 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edda7feb6e555132/documents/GitHub/FEA2D/ver6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{9A4947EE-87E7-4B9F-9D0D-78D81301041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D33804F-9308-47EC-88B5-0D3F1BCAD901}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{9A4947EE-87E7-4B9F-9D0D-78D81301041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83EC7B3D-5E43-4B0A-ABB3-9323970935AE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="340" windowWidth="13420" windowHeight="6560" tabRatio="732" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Load_Condition" sheetId="2" r:id="rId2"/>
+    <sheet name="Elasticity" sheetId="1" r:id="rId1"/>
+    <sheet name="Bound_Condition" sheetId="2" r:id="rId2"/>
     <sheet name="Vertices_Coords" sheetId="3" r:id="rId3"/>
-    <sheet name="Domain_VertID" sheetId="4" r:id="rId4"/>
-    <sheet name="Domain_Cp" sheetId="5" r:id="rId5"/>
+    <sheet name="Domain_Cp" sheetId="5" r:id="rId4"/>
+    <sheet name="Domain_VertID" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Shear modulus [GPa]</t>
   </si>
   <si>
     <t>Poisson's ratio</t>
-  </si>
-  <si>
-    <t>Vertical Loading Displacement [um]</t>
   </si>
   <si>
     <t>Output File Name</t>
@@ -74,6 +71,108 @@
   <si>
     <t>Output_3</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Vertical Loading Displacement [um]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Cp_11</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Cp_12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Cp_22</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>vertex index of P0 at domain bound.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>vertex index of P1 at domain bound.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>vertex index of P2 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P3 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P4 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P5 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P6 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P7 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P8 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P9 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P10 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P11 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P12 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P13 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P14 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P15 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P16 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P17 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P18 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P19 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P20 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P21 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P22 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P23 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P24 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P25 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P26 at domain bound.</t>
+  </si>
+  <si>
+    <t>vertex index of P27 at domain bound.</t>
   </si>
 </sst>
 </file>
@@ -158,6 +257,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,9 +550,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -477,21 +586,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.90625" customWidth="1"/>
+    <col min="1" max="1" width="35.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -499,7 +607,7 @@
         <v>-0.2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -520,21 +628,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -852,326 +963,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8">
-        <v>7</v>
-      </c>
-      <c r="K8">
-        <v>8</v>
-      </c>
-      <c r="L8">
-        <v>9</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="N8">
-        <v>11</v>
-      </c>
-      <c r="O8">
-        <v>12</v>
-      </c>
-      <c r="P8">
-        <v>13</v>
-      </c>
-      <c r="Q8">
-        <v>14</v>
-      </c>
-      <c r="R8">
-        <v>15</v>
-      </c>
-      <c r="S8">
-        <v>27</v>
-      </c>
-      <c r="T8">
-        <v>26</v>
-      </c>
-      <c r="U8">
-        <v>16</v>
-      </c>
-      <c r="V8">
-        <v>17</v>
-      </c>
-      <c r="W8">
-        <v>18</v>
-      </c>
-      <c r="X8">
-        <v>19</v>
-      </c>
-      <c r="Y8">
-        <v>20</v>
-      </c>
-      <c r="Z8">
-        <v>21</v>
-      </c>
-      <c r="AA8">
-        <v>22</v>
-      </c>
-      <c r="AB8">
-        <v>23</v>
-      </c>
-      <c r="AC8">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1.78</v>
@@ -1185,7 +1000,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1.78</v>
@@ -1199,7 +1014,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1.78</v>
@@ -1213,7 +1028,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>1.78</v>
@@ -1227,7 +1042,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1.78</v>
@@ -1241,7 +1056,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1.78</v>
@@ -1255,7 +1070,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1272,4 +1087,300 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AC8"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="29" width="30.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <v>14</v>
+      </c>
+      <c r="R8">
+        <v>15</v>
+      </c>
+      <c r="S8">
+        <v>27</v>
+      </c>
+      <c r="T8">
+        <v>26</v>
+      </c>
+      <c r="U8">
+        <v>16</v>
+      </c>
+      <c r="V8">
+        <v>17</v>
+      </c>
+      <c r="W8">
+        <v>18</v>
+      </c>
+      <c r="X8">
+        <v>19</v>
+      </c>
+      <c r="Y8">
+        <v>20</v>
+      </c>
+      <c r="Z8">
+        <v>21</v>
+      </c>
+      <c r="AA8">
+        <v>22</v>
+      </c>
+      <c r="AB8">
+        <v>23</v>
+      </c>
+      <c r="AC8">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>